<commit_message>
change outcard arrange to horizenal
</commit_message>
<xml_diff>
--- a/doudizhu_layout.xlsx
+++ b/doudizhu_layout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="1160" yWindow="1060" windowWidth="23260" windowHeight="26500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -145,10 +148,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -430,297 +433,297 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="C10" sqref="C10:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="2"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="2" t="s">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="2"/>
+      <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="2"/>
+      <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1" t="s">
         <v>16</v>
@@ -728,20 +731,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="C1:L1"/>
-    <mergeCell ref="G4:I9"/>
-    <mergeCell ref="J4:M9"/>
     <mergeCell ref="N4:O12"/>
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C13:M15"/>
     <mergeCell ref="C10:M12"/>
-    <mergeCell ref="C4:F9"/>
     <mergeCell ref="A4:B12"/>
+    <mergeCell ref="G1:I3"/>
+    <mergeCell ref="C4:G9"/>
+    <mergeCell ref="I4:M9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sound finished changed data storage
</commit_message>
<xml_diff>
--- a/doudizhu_layout.xlsx
+++ b/doudizhu_layout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1060" windowWidth="23260" windowHeight="26500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="26420" yWindow="13680" windowWidth="23260" windowHeight="26500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="斗地主" sheetId="1" r:id="rId1"/>
@@ -468,17 +468,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
@@ -496,16 +496,15 @@
       <c r="M1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -517,14 +516,13 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -536,7 +534,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="3"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">
@@ -706,7 +704,7 @@
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
@@ -727,7 +725,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -745,10 +743,10 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -766,21 +764,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="11">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="G1:I3"/>
+    <mergeCell ref="C4:G9"/>
+    <mergeCell ref="I4:M9"/>
     <mergeCell ref="N4:O12"/>
-    <mergeCell ref="A13:B14"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="C13:M15"/>
     <mergeCell ref="C10:M12"/>
     <mergeCell ref="A4:B12"/>
-    <mergeCell ref="G1:I3"/>
-    <mergeCell ref="C4:G9"/>
-    <mergeCell ref="I4:M9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -791,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>